<commit_message>
added barriers to snail puzzle
</commit_message>
<xml_diff>
--- a/snail-puzzle-template.xlsx
+++ b/snail-puzzle-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliasmead/Documents/GitHub/sins-puzzle-game/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7AB5669-BE08-834E-AE88-4026BCE53809}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC298DC1-7ADA-9E4D-9DE2-793F25374292}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15960" xr2:uid="{472F6002-6B4F-E947-AB59-CF1CF0B20A77}"/>
   </bookViews>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B189FC-6064-A24A-AEFB-A99A578F39D7}">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -913,7 +913,7 @@
       <c r="K42" s="1"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" ht="36" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -922,12 +922,12 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
+      <c r="I43" s="2"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="4"/>
     </row>
-    <row r="44" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="36" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -936,7 +936,7 @@
       <c r="F44" s="6"/>
       <c r="G44" s="14"/>
       <c r="H44" s="1"/>
-      <c r="I44" s="3"/>
+      <c r="I44" s="11"/>
       <c r="J44" s="3"/>
       <c r="K44" s="6"/>
       <c r="L44" s="7"/>

</xml_diff>

<commit_message>
fixed borders on snail puzzle
</commit_message>
<xml_diff>
--- a/snail-puzzle-template.xlsx
+++ b/snail-puzzle-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliasmead/Documents/GitHub/sins-puzzle-game/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC298DC1-7ADA-9E4D-9DE2-793F25374292}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE75683C-C0D1-404F-B48B-C1C4E62FA5DD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15960" xr2:uid="{472F6002-6B4F-E947-AB59-CF1CF0B20A77}"/>
+    <workbookView xWindow="5040" yWindow="940" windowWidth="27640" windowHeight="15960" xr2:uid="{472F6002-6B4F-E947-AB59-CF1CF0B20A77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B189FC-6064-A24A-AEFB-A99A578F39D7}">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -908,12 +908,12 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
+      <c r="I42" s="2"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="36" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -922,12 +922,12 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
-      <c r="I43" s="2"/>
+      <c r="I43" s="4"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="4"/>
     </row>
-    <row r="44" spans="1:12" ht="36" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>

</xml_diff>